<commit_message>
Lots of PDF Report generated Page updated. Fertilizer Recommendations dataset is now fixed. Main GUI Logos added. Small Datasets update.
</commit_message>
<xml_diff>
--- a/Test Reports/5555_test.xlsx
+++ b/Test Reports/5555_test.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T2"/>
+  <dimension ref="A1:U2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -522,6 +522,11 @@
           <t>Recommendations</t>
         </is>
       </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>Fertilizer Recommendation</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -531,22 +536,22 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>19-03-2024</t>
+          <t>24-04-2024</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>232</v>
+        <v>415</v>
       </c>
       <c r="D2" t="n">
-        <v>265</v>
+        <v>321</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>askdjklasjdkl</t>
+          <t>akakjdklasd</t>
         </is>
       </c>
       <c r="F2" t="n">
-        <v>36</v>
+        <v>3</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
@@ -554,48 +559,53 @@
         </is>
       </c>
       <c r="H2" t="n">
-        <v>56</v>
+        <v>25</v>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>26a5sd6a2sdas</t>
+          <t>654asd65asd</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>9895623256</t>
+          <t>8456231231</t>
         </is>
       </c>
       <c r="K2" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="L2" t="n">
-        <v>63</v>
+        <v>250</v>
       </c>
       <c r="M2" t="n">
-        <v>32</v>
+        <v>100</v>
       </c>
       <c r="N2" t="n">
-        <v>326</v>
+        <v>80</v>
       </c>
       <c r="O2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="P2" t="n">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="Q2" t="n">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="R2" t="n">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="S2" t="n">
-        <v>0.4649543563252079</v>
+        <v>0.3625365324113583</v>
       </c>
       <c r="T2" t="inlineStr">
         <is>
-          <t>Millets(Pearl Millet, Sorghum), Maize, Soybean, Groundnut</t>
+          <t>Grow Millets (Sorghum, Pearl millet), Pulses (Pigeon pea, Chickpea), and Oilseeds (Safflower, Castor).</t>
+        </is>
+      </c>
+      <c r="U2" t="inlineStr">
+        <is>
+          <t>Apply organic amendments like Compost (3-5 tonnes/ha), Vermicompost (1.5-2.5 tonnes/ha), or Well-decomposed Farmyard manure (7.5-10 tonnes/ha). Use biofertilizers like Rhizobium (200-300 g/ha), Azotobacter (200-300 g/ha), and Phosphate Solubilizing Bacteria (PSB) (500-750 g/ha). Apply chemical fertilizers at 50% of the recommended dose based on soil test results.</t>
         </is>
       </c>
     </row>

</xml_diff>